<commit_message>
Implement viscous fall simulation with GUI and tests
</commit_message>
<xml_diff>
--- a/lab1/task2.xlsx
+++ b/lab1/task2.xlsx
@@ -256,6 +256,20 @@
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -9137,8 +9151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>